<commit_message>
More corrections on the code
</commit_message>
<xml_diff>
--- a/Search_Results_Google_Shopping.xlsx
+++ b/Search_Results_Google_Shopping.xlsx
@@ -7,21 +7,88 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="iphone 14 pro max 128 gb_Google" sheetId="1" r:id="rId1"/>
+    <sheet name="rtx 4060 ti_Google" sheetId="2" r:id="rId2"/>
+    <sheet name="macbook 16 gb_Google" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>apple iphone 14 pro max 128gb 5g - vitrine - tela super retina xdr oled 6.7 ...</t>
+  </si>
+  <si>
+    <t>apple iphone 14 pro max 128gb dourado 5g tela 6,7" câm. traseira 48+12+12mp frontal 12mp</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?url=https://www.horizonplay.com.br/apple/iphone-de-vitrine/apple-iphone-14-pro-max-128gb-5g-vitrine-tela-super-retina-xdr-oled-6-7%3Fvariant_id%3D22439%26parceiro%3D8926%26srsltid%3DAfmBOopFKy4EOkJzD0HuU6RIDDFK3ueFLXpT8aD5-uju0NhCz5v9LME49fk&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwi18aOTz6ODAxXdpZUCHZoABrwQgOUECKgM&amp;usg=AOvVaw27hg4kgJsPo3lKHhqs56Bk</t>
+  </si>
+  <si>
+    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjeiKqTz6ODAxUyYUgAHbvtAHMYABABGgJjZQ&amp;ase=2&amp;gclid=EAIaIQobChMI3oiqk8-jgwMVMmFIAB277QBzEAQYASABEgIXofD_BwE&amp;sig=AOD64_3dVx6EpiS77leeL_Jas3uaEOLeqw&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwi18aOTz6ODAxXdpZUCHZoABrwQww8I0gs&amp;adurl=</t>
+  </si>
+  <si>
+    <t>placa de vídeo rtx 4060 ti ventus 2x black 8g oc msi nvidia geforce, 8gb gddr6, dlss, ray tracing, g-sync</t>
+  </si>
+  <si>
+    <t>placa de vídeo gigabite nvidia geforce rtx 4060 ti eagle oc 8gb gddr6</t>
+  </si>
+  <si>
+    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiYqvSYz6ODAxXhVUgAHWOZDEoYABADGgJjZQ&amp;ase=2&amp;gclid=EAIaIQobChMImKr0mM-jgwMV4VVIAB1jmQxKEAQYAiABEgLaKvD_BwE&amp;sig=AOD64_0JXG2vcLyJYvnMFLCvK_ehZ_dzog&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwiroe-Yz6ODAxXVqZUCHRlxDmEQww8Ixg0&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005556102900.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwiroe-Yz6ODAxXVqZUCHRlxDmEQguUECO0P&amp;usg=AOvVaw1nXfFDZJrb50Q5t_RskJ85</t>
+  </si>
+  <si>
+    <t>laptop macbook air 2022 com chip m2: tela retina líquida de 13,6 polegadas, 16gb ...</t>
+  </si>
+  <si>
+    <t>macbook air 13.6 m2 256gb 16 ram z15s000ct c/ apple</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005544178685.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwi16vqdz6ODAxUwpJUCHarDBBwQgOUECKQT&amp;usg=AOvVaw2adnxkxO0_0ZYwpKhAN2Jg</t>
+  </si>
+  <si>
+    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjI1_-dz6ODAxWfREgAHT2JANEYABAHGgJjZQ&amp;ase=2&amp;gclid=EAIaIQobChMIyNf_nc-jgwMVn0RIAB09iQDREAQYBCABEgIslfD_BwE&amp;sig=AOD64_2c4LW8m-MAN0Qzivd_Gzw8XPo0jQ&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwi16vqdz6ODAxUwpJUCHarDBBwQww8I3As&amp;adurl=</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -32,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,14 +107,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -340,12 +431,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>5679.06</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>8099</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>2419.99</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>2881.79</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>8952.74</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>10269.5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final tests done, next step: update README.md and add more websites
</commit_message>
<xml_diff>
--- a/Search_Results_Google_Shopping.xlsx
+++ b/Search_Results_Google_Shopping.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0372639560d1acb6/Trabalho/Python/GitHub Desktop/Shopping_Auto_Search/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_B10D180E9152A4B628ED62F0375B123B4B3E6397" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1D7222A-2FB8-4307-993F-038F08355689}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iphone 14 pro max 128 gb_Google" sheetId="1" r:id="rId1"/>
     <sheet name="rtx 4060 ti_Google" sheetId="2" r:id="rId2"/>
     <sheet name="macbook 16 gb_Google" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>Product Name</t>
   </si>
@@ -30,25 +36,106 @@
     <t>apple iphone 14 pro max 128gb 5g - vitrine - tela super retina xdr oled 6.7 ...</t>
   </si>
   <si>
+    <t>apple iphone 14 pro max 128gb roxo-profundo</t>
+  </si>
+  <si>
+    <t>apple iphone 14 pro max (128 gb) - roxo-profundo</t>
+  </si>
+  <si>
+    <t>apple iphone 14 pro max 128gb prateado</t>
+  </si>
+  <si>
     <t>apple iphone 14 pro max 128gb dourado 5g tela 6,7" câm. traseira 48+12+12mp frontal 12mp</t>
   </si>
   <si>
-    <t>https://www.google.com/url?url=https://www.horizonplay.com.br/apple/iphone-de-vitrine/apple-iphone-14-pro-max-128gb-5g-vitrine-tela-super-retina-xdr-oled-6-7%3Fvariant_id%3D22439%26parceiro%3D8926%26srsltid%3DAfmBOopFKy4EOkJzD0HuU6RIDDFK3ueFLXpT8aD5-uju0NhCz5v9LME49fk&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwi18aOTz6ODAxXdpZUCHZoABrwQgOUECKgM&amp;usg=AOvVaw27hg4kgJsPo3lKHhqs56Bk</t>
-  </si>
-  <si>
-    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjeiKqTz6ODAxUyYUgAHbvtAHMYABABGgJjZQ&amp;ase=2&amp;gclid=EAIaIQobChMI3oiqk8-jgwMVMmFIAB277QBzEAQYASABEgIXofD_BwE&amp;sig=AOD64_3dVx6EpiS77leeL_Jas3uaEOLeqw&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwi18aOTz6ODAxXdpZUCHZoABrwQww8I0gs&amp;adurl=</t>
+    <t>apple iphone 14 pro max (128 gb) – dourado</t>
+  </si>
+  <si>
+    <t>iphone 14 pro max 128gb prateado</t>
+  </si>
+  <si>
+    <t>apple iphone 14 pro max 128gb dourado 6,7 48mp, 128gb, dourado, iphone</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?url=https://www.horizonplay.com.br/apple/iphone-de-vitrine/apple-iphone-14-pro-max-128gb-5g-vitrine-tela-super-retina-xdr-oled-6-7%3Fvariant_id%3D22439%26parceiro%3D8926%26srsltid%3DAfmBOoqPussFxSh1eLodHBMrx-G5uYeWYme7F9UYkea3bwSNUZ5r0bg0jtw&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwipm6K81aODAxXbqJUCHSibAycQgOUECOkL&amp;usg=AOvVaw3HLq8h2FwrQfU8dLW8Eory</t>
+  </si>
+  <si>
+    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwje-6a81aODAxV3U0gAHUIvA7MYABAPGgJjZQ&amp;ase=2&amp;gclid=EAIaIQobChMI3vumvNWjgwMVd1NIAB1CLwOzEAQYCCABEgJkLPD_BwE&amp;sig=AOD64_2cPZrpxSNKUJzCgyOeK4gLZ1-mIg&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwipm6K81aODAxXbqJUCHSibAycQww8Iygs&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwje-6a81aODAxV3U0gAHUIvA7MYABALGgJjZQ&amp;ase=2&amp;gclid=EAIaIQobChMI3vumvNWjgwMVd1NIAB1CLwOzEAQYBiABEgI6TvD_BwE&amp;sig=AOD64_0TwDaHgWatqn-fYlhZLQLzLJ-Ghg&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwipm6K81aODAxXbqJUCHSibAycQww8Iwgs&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwje-6a81aODAxV3U0gAHUIvA7MYABARGgJjZQ&amp;ase=2&amp;gclid=EAIaIQobChMI3vumvNWjgwMVd1NIAB1CLwOzEAQYCSABEgLEgfD_BwE&amp;sig=AOD64_3Jwyw5_TL6bBQDqnTArBV48498VQ&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwipm6K81aODAxXbqJUCHSibAycQww8IzQs&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwje-6a81aODAxV3U0gAHUIvA7MYABAdGgJjZQ&amp;ase=2&amp;gclid=EAIaIQobChMI3vumvNWjgwMVd1NIAB1CLwOzEAsYAyABEgLu_vD_BwE&amp;sig=AOD64_1afNHNzON83V0ntZFG01SM6X9hQw&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwipm6K81aODAxXbqJUCHSibAycQ9A4I5xM&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwje-6a81aODAxV3U0gAHUIvA7MYABABGgJjZQ&amp;ase=2&amp;gclid=EAIaIQobChMI3vumvNWjgwMVd1NIAB1CLwOzEAQYASABEgK4X_D_BwE&amp;sig=AOD64_3_LBq_VItFZWoC75gTFbmMiu0JhA&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwipm6K81aODAxXbqJUCHSibAycQww8Irgs&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwje-6a81aODAxV3U0gAHUIvA7MYABADGgJjZQ&amp;ase=2&amp;gclid=EAIaIQobChMI3vumvNWjgwMVd1NIAB1CLwOzEAQYAiABEgJ9k_D_BwE&amp;sig=AOD64_0dbvBW3qdWFo1-1MXUrM7zyhF_rA&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwipm6K81aODAxXbqJUCHSibAycQww8Isgs&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwje-6a81aODAxV3U0gAHUIvA7MYABAFGgJjZQ&amp;ase=2&amp;gclid=EAIaIQobChMI3vumvNWjgwMVd1NIAB1CLwOzEAQYAyABEgJk8PD_BwE&amp;sig=AOD64_3CYz6uPI-9oncUvrJWB-mhKAtSjA&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwipm6K81aODAxXbqJUCHSibAycQww8Itgs&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwje-6a81aODAxV3U0gAHUIvA7MYABAJGgJjZQ&amp;ase=2&amp;gclid=EAIaIQobChMI3vumvNWjgwMVd1NIAB1CLwOzEAQYBSABEgKSCfD_BwE&amp;sig=AOD64_0_oEMBJoB7RRUaDJ12pckztK7n1A&amp;ctype=46&amp;q=&amp;nis=4&amp;ved=0ahUKEwipm6K81aODAxXbqJUCHSibAycQqygIvgs&amp;adurl=</t>
+  </si>
+  <si>
+    <t>placa gráfica geforce-rtx 4060ti, placa de vídeo, x3w, oc, 8gb, 128bit, gddr6 ...</t>
   </si>
   <si>
     <t>placa de vídeo rtx 4060 ti ventus 2x black 8g oc msi nvidia geforce, 8gb gddr6, dlss, ray tracing, g-sync</t>
   </si>
   <si>
+    <t>placa de vídeo rtx 4060 ti ventus 2x black 8g oc msi nvidia geforce, 8</t>
+  </si>
+  <si>
+    <t>placa de vídeo rtx 4060 ti click oc galax nvidia geforce, 8 gb gddr6, dlss, ray tracing - 46isl8md8coc</t>
+  </si>
+  <si>
+    <t>placa de vídeo rtx 4060 ti ex galax nvidia geforce, 8 gb gddr6, dlss, ray tracing - 46isl8md8aex</t>
+  </si>
+  <si>
+    <t>placa de video galax geforce rtx 4060 ti ex 1-click oc, 8gb, gddr6, 128-bit, 46isl8md8aex</t>
+  </si>
+  <si>
+    <t>placa de video galax geforce rtx 4060 ti 1-click oc, 8gb, gddr6, 128-bit, 46isl8md8coc</t>
+  </si>
+  <si>
     <t>placa de vídeo gigabite nvidia geforce rtx 4060 ti eagle oc 8gb gddr6</t>
   </si>
   <si>
-    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiYqvSYz6ODAxXhVUgAHWOZDEoYABADGgJjZQ&amp;ase=2&amp;gclid=EAIaIQobChMImKr0mM-jgwMV4VVIAB1jmQxKEAQYAiABEgLaKvD_BwE&amp;sig=AOD64_0JXG2vcLyJYvnMFLCvK_ehZ_dzog&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwiroe-Yz6ODAxXVqZUCHRlxDmEQww8Ixg0&amp;adurl=</t>
-  </si>
-  <si>
-    <t>https://www.google.com/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005556102900.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwiroe-Yz6ODAxXVqZUCHRlxDmEQguUECO0P&amp;usg=AOvVaw1nXfFDZJrb50Q5t_RskJ85</t>
+    <t>placa de vídeo rtx 4060 ti oc edition asus tuf gaming nvidia geforce, 8 gb gddr6, argb, dlss - tuf-rtx4060ti-o8g-gaming</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005006000031260.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwjvpOPB1aODAxU6q5UCHTESAC8QgOUECMgV&amp;usg=AOvVaw3krcSHVQJQSEv13L8O9OGt</t>
+  </si>
+  <si>
+    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiSvuzB1aODAxU8N60GHZl1AIkYABADGgJwdg&amp;ase=2&amp;gclid=EAIaIQobChMIkr7swdWjgwMVPDetBh2ZdQCJEAQYAiABEgICDPD_BwE&amp;sig=AOD64_0dloao4JS9_i9wI0Dt_tftUqpz4A&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwjvpOPB1aODAxU6q5UCHTESAC8Qww8Ixw0&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiSvuzB1aODAxU8N60GHZl1AIkYABANGgJwdg&amp;ase=2&amp;gclid=EAIaIQobChMIkr7swdWjgwMVPDetBh2ZdQCJEAQYByABEgJpa_D_BwE&amp;sig=AOD64_38NQuiY1gQ-kTS7nORz2V7s1R5GQ&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwjvpOPB1aODAxU6q5UCHTESAC8Qww8I2w0&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiSvuzB1aODAxU8N60GHZl1AIkYABAFGgJwdg&amp;ase=2&amp;gclid=EAIaIQobChMIkr7swdWjgwMVPDetBh2ZdQCJEAQYAyABEgKVtvD_BwE&amp;sig=AOD64_0mVIS8l-p5WPkUJgW6k0lIdf80vw&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwjvpOPB1aODAxU6q5UCHTESAC8Qww8Iyw0&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiSvuzB1aODAxU8N60GHZl1AIkYABAJGgJwdg&amp;ase=2&amp;gclid=EAIaIQobChMIkr7swdWjgwMVPDetBh2ZdQCJEAQYBSABEgJt_fD_BwE&amp;sig=AOD64_2WfDrTvyU0HDSUKKWS3N72KA4Ydw&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwjvpOPB1aODAxU6q5UCHTESAC8Qww8I0w0&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiSvuzB1aODAxU8N60GHZl1AIkYABALGgJwdg&amp;ase=2&amp;gclid=EAIaIQobChMIkr7swdWjgwMVPDetBh2ZdQCJEAQYBiABEgIPKPD_BwE&amp;sig=AOD64_20TfcUorgXaeWctbI2-a1-FStgFg&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwjvpOPB1aODAxU6q5UCHTESAC8Qww8I1w0&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiSvuzB1aODAxU8N60GHZl1AIkYABAPGgJwdg&amp;ase=2&amp;gclid=EAIaIQobChMIkr7swdWjgwMVPDetBh2ZdQCJEAQYCCABEgKYQfD_BwE&amp;sig=AOD64_0ZZALbMhap07VIaR7UMZV688-XBw&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwjvpOPB1aODAxU6q5UCHTESAC8Qww8I3g0&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005556102900.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwjvpOPB1aODAxU6q5UCHTESAC8QguUECO4P&amp;usg=AOvVaw0hIGsgA2jiUfnEgs3XWLNN</t>
+  </si>
+  <si>
+    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwiSvuzB1aODAxU8N60GHZl1AIkYABAHGgJwdg&amp;ase=2&amp;gclid=EAIaIQobChMIkr7swdWjgwMVPDetBh2ZdQCJEAQYBCABEgJQCfD_BwE&amp;sig=AOD64_1vHLoKnM69xPY49v0UFo48VBOXDQ&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwjvpOPB1aODAxU6q5UCHTESAC8Qww8Izw0&amp;adurl=</t>
   </si>
   <si>
     <t>laptop macbook air 2022 com chip m2: tela retina líquida de 13,6 polegadas, 16gb ...</t>
@@ -57,17 +144,23 @@
     <t>macbook air 13.6 m2 256gb 16 ram z15s000ct c/ apple</t>
   </si>
   <si>
-    <t>https://www.google.com/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005544178685.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwi16vqdz6ODAxUwpJUCHarDBBwQgOUECKQT&amp;usg=AOvVaw2adnxkxO0_0ZYwpKhAN2Jg</t>
-  </si>
-  <si>
-    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwjI1_-dz6ODAxWfREgAHT2JANEYABAHGgJjZQ&amp;ase=2&amp;gclid=EAIaIQobChMIyNf_nc-jgwMVn0RIAB09iQDREAQYBCABEgIslfD_BwE&amp;sig=AOD64_2c4LW8m-MAN0Qzivd_Gzw8XPo0jQ&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwi16vqdz6ODAxUwpJUCHarDBBwQww8I3As&amp;adurl=</t>
+    <t>macbook pro mkgp3/m1/16gb ram/ 512gb ssd/ 14,2 (2021) apple</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?url=https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005005544178685.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;opi=95576897&amp;sa=U&amp;ved=0ahUKEwjey97G1aODAxUns5UCHdU8A0cQgOUECLES&amp;usg=AOvVaw3QHk1LsK2hNu6-mfJEgdeY</t>
+  </si>
+  <si>
+    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwia2OLG1aODAxWhQkgAHbxiAG0YABALGgJjZQ&amp;ase=2&amp;gclid=EAIaIQobChMImtjixtWjgwMVoUJIAB28YgBtEAQYBiABEgJonPD_BwE&amp;sig=AOD64_0Aw3QuDRbz7iLIlWkjnIqSgbZ4VA&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwjey97G1aODAxUns5UCHdU8A0cQww8Itgs&amp;adurl=</t>
+  </si>
+  <si>
+    <t>https://www.google.com/aclk?sa=l&amp;ai=DChcSEwia2OLG1aODAxWhQkgAHbxiAG0YABANGgJjZQ&amp;ase=2&amp;gclid=EAIaIQobChMImtjixtWjgwMVoUJIAB28YgBtEAQYByABEgKe7PD_BwE&amp;sig=AOD64_3BISNWqs64Mp7pjLPViu1Rx6aSyA&amp;ctype=5&amp;q=&amp;nis=4&amp;ved=0ahUKEwjey97G1aODAxUns5UCHdU8A0cQww8Iuws&amp;adurl=</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,18 +231,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -187,7 +288,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -221,6 +322,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -255,9 +357,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -430,14 +533,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="83.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,7 +554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -456,38 +562,127 @@
         <v>5679.06</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
+        <v>7543.8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>7900</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>7900</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>7900</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
         <v>8099</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>8199</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>8199</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>8369.1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="105.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -498,46 +693,135 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B2">
-        <v>2419.99</v>
+        <v>2414.25</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B3">
+        <v>2419.9899999999998</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>2419.9899999999998</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>2499.9899999999998</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>2599.9899999999998</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>2599.9899999999998</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>2599.9899999999998</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9">
         <v>2881.79</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
+      <c r="C9" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>2899.99</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="76" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,32 +832,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>8952.74</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>10269.5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4">
+        <v>10499</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>